<commit_message>
Update Supplemental Table 1
</commit_message>
<xml_diff>
--- a/Supplemental_Files/SupplTable1_PeakNumbers_FINAL.xlsx
+++ b/Supplemental_Files/SupplTable1_PeakNumbers_FINAL.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <r>
       <rPr>
@@ -28,6 +28,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Table 1.</t>
     </r>
@@ -36,6 +37,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">: Peak numbers in barley embryo ChIP-seq and ATAC-seq datasets</t>
     </r>
@@ -174,6 +176,42 @@
   </si>
   <si>
     <t xml:space="preserve">Morex24DAP_ATACseq_intersect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intergenic peaks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtered using “Coding potential set of 77364 regions including HC and LC genes, lncRNA candidates and RNA-seq positive regions”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMRs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intergenic_4DAG_ATACseq_merged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intergenic_8DAP_ATACseq_intersect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intergenic_24DAP_ATACseq_intersect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intergenic_Leaf_pooledReps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intergenic</t>
   </si>
 </sst>
 </file>
@@ -183,11 +221,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -209,9 +248,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,7 +278,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB4C7DC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE994"/>
+        <bgColor rgb="FFFFFFA6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFB4C7DC"/>
       </patternFill>
     </fill>
   </fills>
@@ -272,44 +341,76 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -338,7 +439,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB4C7DC"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -347,7 +448,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -360,10 +461,10 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFFA6"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFE994"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -496,355 +597,544 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="30.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="12" style="0" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="28.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="11.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="30.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="12" style="1" width="11.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="6" t="n">
         <v>54098</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="6" t="n">
+      <c r="C3" s="4"/>
+      <c r="D3" s="7" t="n">
         <v>61885</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="6" t="n">
+      <c r="F3" s="4"/>
+      <c r="G3" s="7" t="n">
         <v>53653</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="6" t="n">
+      <c r="I3" s="4"/>
+      <c r="J3" s="7" t="n">
         <v>71668</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="6" t="n">
         <v>29863</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="6" t="n">
+      <c r="C4" s="4"/>
+      <c r="D4" s="7" t="n">
         <v>30178</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="6" t="n">
+      <c r="F4" s="4"/>
+      <c r="G4" s="7" t="n">
         <v>48396</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="6" t="n">
+      <c r="I4" s="4"/>
+      <c r="J4" s="7" t="n">
         <v>85421</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="6" t="n">
         <v>10627</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="6" t="n">
+      <c r="C5" s="4"/>
+      <c r="D5" s="7" t="n">
         <v>25994</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="6" t="n">
+      <c r="F5" s="4"/>
+      <c r="G5" s="7" t="n">
         <v>46140</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="6" t="n">
+      <c r="I5" s="4"/>
+      <c r="J5" s="7" t="n">
         <v>70564</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="6" t="n">
         <v>73333</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="7" t="n">
         <v>22130</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="6" t="n">
+      <c r="F7" s="4"/>
+      <c r="G7" s="7" t="n">
         <v>12976</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="6" t="n">
+      <c r="I7" s="4"/>
+      <c r="J7" s="7" t="n">
         <v>46915</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="6" t="n">
         <v>53303</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="7" t="n">
         <v>26393</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="6" t="n">
+      <c r="F8" s="4"/>
+      <c r="G8" s="7" t="n">
         <v>16198</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="6" t="n">
+      <c r="I8" s="4"/>
+      <c r="J8" s="7" t="n">
         <v>43595</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="6" t="n">
         <v>55758</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="7" t="n">
         <v>15911</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="6" t="n">
+      <c r="F9" s="4"/>
+      <c r="G9" s="7" t="n">
         <v>10075</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="6" t="n">
+      <c r="I9" s="4"/>
+      <c r="J9" s="7" t="n">
         <v>38506</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="6" t="n">
         <v>42899</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="7" t="n">
         <v>32119</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="6" t="n">
+      <c r="F11" s="4"/>
+      <c r="G11" s="7" t="n">
         <v>47454</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="6" t="n">
+      <c r="I11" s="4"/>
+      <c r="J11" s="7" t="n">
         <v>59006</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="K11" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="6" t="n">
         <v>145943</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="6" t="n">
+      <c r="D12" s="7" t="n">
         <v>66104</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="6" t="n">
+      <c r="F12" s="4"/>
+      <c r="G12" s="7" t="n">
         <v>51563</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="6" t="n">
+      <c r="I12" s="4"/>
+      <c r="J12" s="7" t="n">
         <v>51373</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="6" t="n">
         <v>127166</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="7" t="n">
         <v>30159</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="6" t="n">
+      <c r="F13" s="4"/>
+      <c r="G13" s="7" t="n">
         <v>46220</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="6" t="n">
+      <c r="I13" s="4"/>
+      <c r="J13" s="7" t="n">
         <v>48316</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="K13" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
+      <c r="A14" s="6" t="n">
         <v>93441</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>45</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="n">
+        <v>43851</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13" t="n">
+        <v>14436</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14" t="n">
+        <v>4396</v>
+      </c>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7" t="n">
+        <v>2385</v>
+      </c>
+    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="9"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="n">
+        <v>23453</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="15" t="n">
+        <v>12487</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14" t="n">
+        <v>3970</v>
+      </c>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7" t="n">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="n">
+        <v>58823</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13" t="n">
+        <v>19039</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14" t="n">
+        <v>6005</v>
+      </c>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7" t="n">
+        <v>3403</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8"/>
+      <c r="B24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="n">
+        <v>32955</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13" t="n">
+        <v>20540</v>
+      </c>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14" t="n">
+        <v>6542</v>
+      </c>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7" t="n">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="17"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="17" t="n">
+        <v>139283</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="17" t="n">
+        <v>74614</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>